<commit_message>
updated laws dataset and color bar
</commit_message>
<xml_diff>
--- a/myapp/data/regulations_information.xlsx
+++ b/myapp/data/regulations_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviaberreby/Desktop/ES96/MAP/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviaberreby/Desktop/ES96/myapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1339D9-B2F5-9A4C-A6FA-187CEA043CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438A5B45-5B08-7443-922C-5C43566239DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,7 +797,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -944,14 +944,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1074,10 +1066,10 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1299,7 +1291,7 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1315,13 +1307,13 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>200</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">

</xml_diff>